<commit_message>
Colocando a coluna de mes ano
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,11 @@
       <c r="D1" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -463,6 +468,11 @@
           <t>264.160,51</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -483,6 +493,11 @@
           <t>264.160,51</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -503,6 +518,11 @@
           <t>264.160,51</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -523,6 +543,11 @@
           <t>39.500,05</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -543,6 +568,11 @@
           <t>14.000,00</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -563,6 +593,11 @@
           <t>600,00</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -583,6 +618,11 @@
           <t>24.158,05</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -603,6 +643,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -623,6 +668,11 @@
           <t>742,00</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -643,6 +693,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -663,6 +718,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -683,6 +743,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -703,6 +768,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -723,6 +793,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -743,6 +818,11 @@
           <t>222.582,37</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -763,6 +843,11 @@
           <t>132.686,07</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -783,6 +868,11 @@
           <t>15.850,00</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -803,6 +893,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -823,6 +918,11 @@
           <t>22.991,89</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -843,6 +943,11 @@
           <t>48.954,41</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -863,6 +968,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -883,6 +993,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -903,6 +1018,11 @@
           <t>2.100,00</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -923,6 +1043,11 @@
           <t>1.753,09</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -943,6 +1068,11 @@
           <t>1.434,44</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -963,6 +1093,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -983,6 +1118,11 @@
           <t>318,65</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1003,6 +1143,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1023,6 +1168,11 @@
           <t>325,00</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1043,6 +1193,11 @@
           <t>325,00</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1063,6 +1218,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1083,6 +1243,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1103,6 +1268,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1123,6 +1293,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1143,6 +1318,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1163,6 +1343,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1183,6 +1368,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1203,6 +1393,11 @@
           <t>264.160,51</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1223,6 +1418,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1243,6 +1443,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1263,6 +1468,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1283,6 +1493,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1303,6 +1518,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1323,6 +1543,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1343,6 +1568,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1363,6 +1593,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1383,6 +1618,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1403,6 +1643,11 @@
           <t>264.160,51</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1423,6 +1668,11 @@
           <t>220.652,86</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1443,6 +1693,11 @@
           <t>220.652,86</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1463,6 +1718,11 @@
           <t>77.307,73</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1483,6 +1743,11 @@
           <t>36.523,78</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1503,6 +1768,11 @@
           <t>2.230,82</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1523,6 +1793,11 @@
           <t>687,07</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1543,6 +1818,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1563,6 +1843,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1583,6 +1868,11 @@
           <t>2.271,21</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1603,6 +1893,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1623,6 +1918,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1643,6 +1943,11 @@
           <t>7.719,85</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1663,6 +1968,11 @@
           <t>1.558,77</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1683,6 +1993,11 @@
           <t>3.318,53</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1703,6 +2018,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1723,6 +2043,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1743,6 +2068,11 @@
           <t>11.259,43</t>
         </is>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1763,6 +2093,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1783,6 +2118,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1803,6 +2143,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1823,6 +2168,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1843,6 +2193,11 @@
           <t>11.267,11</t>
         </is>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1863,6 +2218,11 @@
           <t>424,88</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1883,6 +2243,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1903,6 +2268,11 @@
           <t>46,28</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1923,6 +2293,11 @@
           <t>10.474,27</t>
         </is>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1943,6 +2318,11 @@
           <t>7.180,00</t>
         </is>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -1963,6 +2343,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -1983,6 +2368,11 @@
           <t>3.294,27</t>
         </is>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2003,6 +2393,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2023,6 +2418,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2043,6 +2443,11 @@
           <t>112.015,79</t>
         </is>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2063,6 +2468,11 @@
           <t>18.377,43</t>
         </is>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2083,6 +2493,11 @@
           <t>12.788,90</t>
         </is>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2103,6 +2518,11 @@
           <t>390,69</t>
         </is>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2123,6 +2543,11 @@
           <t>144,09</t>
         </is>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2143,6 +2568,11 @@
           <t>12.397,74</t>
         </is>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2163,6 +2593,11 @@
           <t>332,50</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2183,6 +2618,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2203,6 +2643,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2223,6 +2668,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2243,6 +2693,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2263,6 +2718,11 @@
           <t>292,13</t>
         </is>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2283,6 +2743,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2303,6 +2768,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2323,6 +2793,11 @@
           <t>16.390,00</t>
         </is>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2343,6 +2818,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2363,6 +2843,11 @@
           <t>106,50</t>
         </is>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2383,6 +2868,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -2403,6 +2893,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2423,6 +2918,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2443,6 +2943,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2463,6 +2968,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -2483,6 +2993,11 @@
           <t>1.450,00</t>
         </is>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -2503,6 +3018,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -2523,6 +3043,11 @@
           <t>2.332,12</t>
         </is>
       </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -2543,6 +3068,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -2563,6 +3093,11 @@
           <t>4.195,83</t>
         </is>
       </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -2583,6 +3118,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -2603,6 +3143,11 @@
           <t>18.157,45</t>
         </is>
       </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -2623,6 +3168,11 @@
           <t>3.550,00</t>
         </is>
       </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -2643,6 +3193,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -2663,6 +3218,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -2683,6 +3243,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -2703,6 +3268,11 @@
           <t>6.500,00</t>
         </is>
       </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -2723,6 +3293,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -2743,6 +3318,11 @@
           <t>260,79</t>
         </is>
       </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -2763,6 +3343,11 @@
           <t>14.349,62</t>
         </is>
       </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -2783,6 +3368,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -2803,6 +3393,11 @@
           <t>114,16</t>
         </is>
       </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -2823,6 +3418,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -2843,6 +3443,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -2863,6 +3468,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -2883,6 +3493,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -2903,6 +3518,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -2923,6 +3543,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -2943,6 +3568,11 @@
           <t>75,83</t>
         </is>
       </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -2963,6 +3593,11 @@
           <t>38,33</t>
         </is>
       </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -2983,6 +3618,11 @@
           <t>20.740,91</t>
         </is>
       </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -3003,6 +3643,11 @@
           <t>2.904,71</t>
         </is>
       </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -3023,6 +3668,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -3043,6 +3693,11 @@
           <t>692,29</t>
         </is>
       </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -3063,6 +3718,11 @@
           <t>17.143,91</t>
         </is>
       </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -3083,6 +3743,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -3103,6 +3768,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -3123,6 +3793,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -3143,6 +3818,11 @@
           <t>43.507,65</t>
         </is>
       </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -3163,6 +3843,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -3183,6 +3868,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -3203,6 +3893,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -3223,6 +3918,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -3243,6 +3943,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -3263,6 +3968,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -3283,6 +3993,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -3303,6 +4018,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -3323,6 +4043,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -3343,6 +4068,11 @@
           <t>43.507,65</t>
         </is>
       </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -3363,6 +4093,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -3383,6 +4118,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -3403,6 +4143,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -3423,6 +4168,11 @@
           <t>0,00</t>
         </is>
       </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -3441,6 +4191,11 @@
       <c r="D151" t="inlineStr">
         <is>
           <t>43.507,65</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Abr-24</t>
         </is>
       </c>
     </row>

</xml_diff>